<commit_message>
Graphs updated in LPInstance_Tet.xlsx
</commit_message>
<xml_diff>
--- a/LinearProgramming/LPInstance_test.xlsx
+++ b/LinearProgramming/LPInstance_test.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="LPInstance_test" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -709,15 +709,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>LPInstance_test!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Apache total</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>SimplexApache</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575">
@@ -939,15 +931,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>LPInstance_test!$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v> SampLP Simplex</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>SampLP</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575">
@@ -1169,15 +1153,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:strRef>
-              <c:f>LPInstance_test!$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v> IterSampLP Simplex</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>IterSampLP</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575">
@@ -1395,11 +1371,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87476480"/>
-        <c:axId val="87474944"/>
+        <c:axId val="76510720"/>
+        <c:axId val="76512640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87476480"/>
+        <c:axId val="76510720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1424,12 +1400,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87474944"/>
+        <c:crossAx val="76512640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87474944"/>
+        <c:axId val="76512640"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1454,9 +1430,9 @@
           </c:tx>
           <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87476480"/>
+        <c:crossAx val="76510720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1469,7 +1445,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1945,11 +1921,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="81119872"/>
-        <c:axId val="81118336"/>
+        <c:axId val="88142208"/>
+        <c:axId val="91172864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81119872"/>
+        <c:axId val="88142208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1974,12 +1950,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81118336"/>
+        <c:crossAx val="91172864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81118336"/>
+        <c:axId val="91172864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1987,7 +1963,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81119872"/>
+        <c:crossAx val="88142208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2000,7 +1976,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2703,11 +2679,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="81480320"/>
-        <c:axId val="81478784"/>
+        <c:axId val="100600832"/>
+        <c:axId val="128524288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81480320"/>
+        <c:axId val="100600832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2732,12 +2708,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81478784"/>
+        <c:crossAx val="128524288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81478784"/>
+        <c:axId val="128524288"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2762,9 +2738,9 @@
           </c:tx>
           <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81480320"/>
+        <c:crossAx val="100600832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2777,7 +2753,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3235,23 +3211,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="112675072"/>
-        <c:axId val="112673152"/>
+        <c:axId val="143829248"/>
+        <c:axId val="143905152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="112675072"/>
+        <c:axId val="143829248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112673152"/>
+        <c:crossAx val="143905152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="112673152"/>
+        <c:axId val="143905152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3259,7 +3235,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112675072"/>
+        <c:crossAx val="143829248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3272,7 +3248,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3313,15 +3289,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>495299</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>247649</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>295274</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>47624</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3343,14 +3319,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3690,8 +3666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="D35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O47" sqref="O47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Table 2 added to the report
</commit_message>
<xml_diff>
--- a/LinearProgramming/LPInstance_test.xlsx
+++ b/LinearProgramming/LPInstance_test.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LPInstance_test" sheetId="1" r:id="rId1"/>
+    <sheet name="Blad1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>Instance</t>
   </si>
@@ -3666,8 +3667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O47" sqref="O47"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5052,4 +5053,874 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1250</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>91605</v>
+      </c>
+      <c r="E2">
+        <v>8571</v>
+      </c>
+      <c r="F2">
+        <v>3663</v>
+      </c>
+      <c r="G2">
+        <v>93396</v>
+      </c>
+      <c r="H2">
+        <v>8672</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1250</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>190610</v>
+      </c>
+      <c r="E3">
+        <v>17437</v>
+      </c>
+      <c r="F3">
+        <v>10941</v>
+      </c>
+      <c r="G3">
+        <v>189220</v>
+      </c>
+      <c r="H3">
+        <v>38456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1250</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>5599</v>
+      </c>
+      <c r="E4">
+        <v>2080</v>
+      </c>
+      <c r="F4">
+        <v>181</v>
+      </c>
+      <c r="G4">
+        <v>17335</v>
+      </c>
+      <c r="H4">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1250</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>59826</v>
+      </c>
+      <c r="E5">
+        <v>6676</v>
+      </c>
+      <c r="F5">
+        <v>2950</v>
+      </c>
+      <c r="G5">
+        <v>75248</v>
+      </c>
+      <c r="H5">
+        <v>8101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>2160</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>266887</v>
+      </c>
+      <c r="E6">
+        <v>24334</v>
+      </c>
+      <c r="F6">
+        <v>13178</v>
+      </c>
+      <c r="G6">
+        <v>301377</v>
+      </c>
+      <c r="H6">
+        <v>43118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>2160</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>269059</v>
+      </c>
+      <c r="E7">
+        <v>24017</v>
+      </c>
+      <c r="F7">
+        <v>13366</v>
+      </c>
+      <c r="G7">
+        <v>291398</v>
+      </c>
+      <c r="H7">
+        <v>45011</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>2160</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>434566</v>
+      </c>
+      <c r="E8">
+        <v>21049</v>
+      </c>
+      <c r="F8">
+        <v>11186</v>
+      </c>
+      <c r="G8">
+        <v>231637</v>
+      </c>
+      <c r="H8">
+        <v>25728</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>2160</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>182747</v>
+      </c>
+      <c r="E9">
+        <v>17205</v>
+      </c>
+      <c r="F9">
+        <v>8382</v>
+      </c>
+      <c r="G9">
+        <v>192605</v>
+      </c>
+      <c r="H9">
+        <v>22020</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>270</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>3518</v>
+      </c>
+      <c r="E10">
+        <v>843</v>
+      </c>
+      <c r="F10">
+        <v>482</v>
+      </c>
+      <c r="G10">
+        <v>6767</v>
+      </c>
+      <c r="H10">
+        <v>1663</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>270</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>2498</v>
+      </c>
+      <c r="E11">
+        <v>627</v>
+      </c>
+      <c r="F11">
+        <v>314</v>
+      </c>
+      <c r="G11">
+        <v>4419</v>
+      </c>
+      <c r="H11">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>270</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>1249</v>
+      </c>
+      <c r="E12">
+        <v>449</v>
+      </c>
+      <c r="F12">
+        <v>189</v>
+      </c>
+      <c r="G12">
+        <v>2677</v>
+      </c>
+      <c r="H12">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>270</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>2591</v>
+      </c>
+      <c r="E13">
+        <v>681</v>
+      </c>
+      <c r="F13">
+        <v>353</v>
+      </c>
+      <c r="G13">
+        <v>5213</v>
+      </c>
+      <c r="H13">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>3430</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>1402486</v>
+      </c>
+      <c r="E14">
+        <v>56464</v>
+      </c>
+      <c r="F14">
+        <v>31761</v>
+      </c>
+      <c r="G14">
+        <v>650137</v>
+      </c>
+      <c r="H14">
+        <v>86166</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>3430</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>805804</v>
+      </c>
+      <c r="E15">
+        <v>57138</v>
+      </c>
+      <c r="F15">
+        <v>29486</v>
+      </c>
+      <c r="G15">
+        <v>685525</v>
+      </c>
+      <c r="H15">
+        <v>85931</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>3430</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <v>1209336</v>
+      </c>
+      <c r="E16">
+        <v>55658</v>
+      </c>
+      <c r="F16">
+        <v>27997</v>
+      </c>
+      <c r="G16">
+        <v>753164</v>
+      </c>
+      <c r="H16">
+        <v>86389</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>3430</v>
+      </c>
+      <c r="C17">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <v>1349811</v>
+      </c>
+      <c r="E17">
+        <v>67305</v>
+      </c>
+      <c r="F17">
+        <v>35871</v>
+      </c>
+      <c r="G17">
+        <v>950145</v>
+      </c>
+      <c r="H17">
+        <v>130263</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>5120</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <v>2087614</v>
+      </c>
+      <c r="E18">
+        <v>86721</v>
+      </c>
+      <c r="F18">
+        <v>32143</v>
+      </c>
+      <c r="G18">
+        <v>1428837</v>
+      </c>
+      <c r="H18">
+        <v>130015</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>5120</v>
+      </c>
+      <c r="C19">
+        <v>8</v>
+      </c>
+      <c r="D19">
+        <v>2891915</v>
+      </c>
+      <c r="E19">
+        <v>87656</v>
+      </c>
+      <c r="F19">
+        <v>36512</v>
+      </c>
+      <c r="G19">
+        <v>1643975</v>
+      </c>
+      <c r="H19">
+        <v>171009</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>5120</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20">
+        <v>1170917</v>
+      </c>
+      <c r="E20">
+        <v>71039</v>
+      </c>
+      <c r="F20">
+        <v>28429</v>
+      </c>
+      <c r="G20">
+        <v>797186</v>
+      </c>
+      <c r="H20">
+        <v>68344</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>5120</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21">
+        <v>1545349</v>
+      </c>
+      <c r="E21">
+        <v>78305</v>
+      </c>
+      <c r="F21">
+        <v>23893</v>
+      </c>
+      <c r="G21">
+        <v>1470287</v>
+      </c>
+      <c r="H21">
+        <v>101232</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>640</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>24974</v>
+      </c>
+      <c r="E22">
+        <v>3044</v>
+      </c>
+      <c r="F22">
+        <v>1815</v>
+      </c>
+      <c r="G22">
+        <v>27322</v>
+      </c>
+      <c r="H22">
+        <v>4874</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>640</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <v>23685</v>
+      </c>
+      <c r="E23">
+        <v>2223</v>
+      </c>
+      <c r="F23">
+        <v>1317</v>
+      </c>
+      <c r="G23">
+        <v>19794</v>
+      </c>
+      <c r="H23">
+        <v>3663</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>640</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>12578</v>
+      </c>
+      <c r="E24">
+        <v>2169</v>
+      </c>
+      <c r="F24">
+        <v>1250</v>
+      </c>
+      <c r="G24">
+        <v>18999</v>
+      </c>
+      <c r="H24">
+        <v>3526</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25">
+        <v>640</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>17826</v>
+      </c>
+      <c r="E25">
+        <v>2374</v>
+      </c>
+      <c r="F25">
+        <v>1348</v>
+      </c>
+      <c r="G25">
+        <v>25389</v>
+      </c>
+      <c r="H25">
+        <v>4220</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>7290</v>
+      </c>
+      <c r="C26">
+        <v>9</v>
+      </c>
+      <c r="D26">
+        <v>8944001</v>
+      </c>
+      <c r="E26">
+        <v>252987</v>
+      </c>
+      <c r="F26">
+        <v>95365</v>
+      </c>
+      <c r="G26">
+        <v>5591116</v>
+      </c>
+      <c r="H26">
+        <v>751477</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27">
+        <v>7290</v>
+      </c>
+      <c r="C27">
+        <v>9</v>
+      </c>
+      <c r="D27">
+        <v>3770595</v>
+      </c>
+      <c r="E27">
+        <v>171645</v>
+      </c>
+      <c r="F27">
+        <v>31653</v>
+      </c>
+      <c r="G27">
+        <v>4177553</v>
+      </c>
+      <c r="H27">
+        <v>267840</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28">
+        <v>7290</v>
+      </c>
+      <c r="C28">
+        <v>9</v>
+      </c>
+      <c r="D28">
+        <v>2190897</v>
+      </c>
+      <c r="E28">
+        <v>171699</v>
+      </c>
+      <c r="F28">
+        <v>28134</v>
+      </c>
+      <c r="G28">
+        <v>3349625</v>
+      </c>
+      <c r="H28">
+        <v>210678</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29">
+        <v>7290</v>
+      </c>
+      <c r="C29">
+        <v>9</v>
+      </c>
+      <c r="D29">
+        <v>4572966</v>
+      </c>
+      <c r="E29">
+        <v>201903</v>
+      </c>
+      <c r="F29">
+        <v>45554</v>
+      </c>
+      <c r="G29">
+        <v>4859949</v>
+      </c>
+      <c r="H29">
+        <v>348285</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <v>80</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>31</v>
+      </c>
+      <c r="E30">
+        <v>25</v>
+      </c>
+      <c r="F30">
+        <v>10</v>
+      </c>
+      <c r="G30">
+        <v>127</v>
+      </c>
+      <c r="H30">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31">
+        <v>80</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>106</v>
+      </c>
+      <c r="E31">
+        <v>57</v>
+      </c>
+      <c r="F31">
+        <v>30</v>
+      </c>
+      <c r="G31">
+        <v>255</v>
+      </c>
+      <c r="H31">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32">
+        <v>80</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>31</v>
+      </c>
+      <c r="E32">
+        <v>25</v>
+      </c>
+      <c r="F32">
+        <v>9</v>
+      </c>
+      <c r="G32">
+        <v>135</v>
+      </c>
+      <c r="H32">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33">
+        <v>4</v>
+      </c>
+      <c r="B33">
+        <v>80</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>31</v>
+      </c>
+      <c r="E33">
+        <v>25</v>
+      </c>
+      <c r="F33">
+        <v>10</v>
+      </c>
+      <c r="G33">
+        <v>128</v>
+      </c>
+      <c r="H33">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>